<commit_message>
capitalized the Type records
</commit_message>
<xml_diff>
--- a/legacy/clean/type.xlsx
+++ b/legacy/clean/type.xlsx
@@ -443,14 +443,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tablet</t>
+          <t>Tablet</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>syrup</t>
+          <t>Syrup</t>
         </is>
       </c>
     </row>

</xml_diff>